<commit_message>
fix bugs when send mails
</commit_message>
<xml_diff>
--- a/uploads/status-by-agent/agent.xlsx
+++ b/uploads/status-by-agent/agent.xlsx
@@ -32,8 +32,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -397,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -433,230 +434,146 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>חידושים לא אוטומטי</v>
+        <v>מיגיר</v>
       </c>
       <c r="B2" t="str">
-        <v>?</v>
+        <v>לוייב</v>
       </c>
       <c r="C2" t="str">
-        <v>-</v>
+        <v xml:space="preserve">הצעה </v>
       </c>
       <c r="D2" t="str">
         <v>גל מסיקה</v>
       </c>
       <c r="E2" t="str">
-        <v>ברקוביץ הדסה</v>
+        <v>לוי הודיה</v>
       </c>
       <c r="F2" t="str">
-        <v>-</v>
+        <v>בוצע חישוב לא זכאי להחזר</v>
       </c>
       <c r="G2" t="str">
-        <v>23.01.2024</v>
+        <v>30.03.2023</v>
       </c>
       <c r="H2" t="str">
-        <v>03.03.2024</v>
+        <v>12.02.2024</v>
       </c>
       <c r="I2" t="str">
-        <v>אלמנטר</v>
+        <v>החזרי מס</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>חיה</v>
+        <v>אלבר ואילנית*</v>
       </c>
       <c r="B3" t="str">
-        <v>בן שושן</v>
+        <v>דהן</v>
       </c>
       <c r="C3" t="str">
-        <v>-</v>
+        <v>הופק</v>
       </c>
       <c r="D3" t="str">
         <v>גל מסיקה</v>
       </c>
       <c r="E3" t="str">
-        <v>ברקוביץ הדסה</v>
+        <v>יהוד ספיר</v>
       </c>
       <c r="F3" t="str">
-        <v>לגבי שם סוכן -יתכן ששיכת לאיציק -לבדוק</v>
+        <v>בוצע גבייה 12.12.23בוצע גבייה 14.02.24</v>
       </c>
       <c r="G3" t="str">
-        <v>08.02.2024</v>
+        <v>14.05.2023</v>
       </c>
       <c r="H3" t="str">
-        <v>08.02.2024</v>
+        <v>18.02.2024</v>
       </c>
       <c r="I3" t="str">
-        <v>אלמנטר</v>
+        <v>החזרי מס</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>מור לוי</v>
+        <v>אוריה</v>
       </c>
       <c r="B4" t="str">
-        <v>עסק</v>
+        <v>לברון</v>
       </c>
       <c r="C4" t="str">
-        <v>אין מענה</v>
+        <v xml:space="preserve">הצעה </v>
       </c>
       <c r="D4" t="str">
         <v>גל מסיקה</v>
       </c>
       <c r="E4" t="str">
-        <v>ברנד שולמית</v>
+        <v>עוזירי קארין</v>
       </c>
       <c r="F4" t="str">
-        <v>-</v>
+        <v>בוצע חישוב - לא זכאי להחזר</v>
       </c>
       <c r="G4" t="str">
-        <v>11.02.2024</v>
+        <v>22.08.2023</v>
       </c>
       <c r="H4" t="str">
-        <v>11.02.2024</v>
+        <v>14.01.2024</v>
       </c>
       <c r="I4" t="str">
-        <v>אלמנטר</v>
+        <v>החזרי מס</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>דניאל</v>
+        <v>אלירז ( עידן )</v>
       </c>
       <c r="B5" t="str">
-        <v>מלץ</v>
+        <v>כס</v>
       </c>
       <c r="C5" t="str">
-        <v>-</v>
+        <v>הצעה</v>
       </c>
       <c r="D5" t="str">
         <v>גל מסיקה</v>
       </c>
       <c r="E5" t="str">
-        <v>חן אביגיל</v>
+        <v xml:space="preserve">כהן ליאל </v>
       </c>
       <c r="F5" t="str">
-        <v>שאול 3 חיפה קומה 3 מתוך 3</v>
+        <v>-</v>
       </c>
       <c r="G5" t="str">
-        <v>14.02.2024</v>
+        <v>23.08.2023</v>
       </c>
       <c r="H5" t="str">
-        <v>15.02.2024</v>
-      </c>
-      <c r="I5" t="str">
-        <v>אלמנטר</v>
+        <v>12.02.2024</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>עליזה</v>
+        <v>עידן ( ואלירז )</v>
       </c>
       <c r="B6" t="str">
-        <v>איתני</v>
+        <v>כס</v>
       </c>
       <c r="C6" t="str">
-        <v xml:space="preserve">הצעה </v>
+        <v>הצעה</v>
       </c>
       <c r="D6" t="str">
         <v>גל מסיקה</v>
       </c>
       <c r="E6" t="str">
-        <v>דהן גלית</v>
+        <v>גרינברגר גילי</v>
       </c>
       <c r="F6" t="str">
-        <v>-</v>
+        <v>בתהליך חישוב חוזר 25.05.24</v>
       </c>
       <c r="G6" t="str">
-        <v>13.03.2024</v>
+        <v>28.08.2023</v>
       </c>
       <c r="H6" t="str">
-        <v>13.03.2024</v>
-      </c>
-      <c r="I6" t="str">
-        <v>פקדונות/משכנתא/הלוואות</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>אבי</v>
-      </c>
-      <c r="B7" t="str">
-        <v>עזרא</v>
-      </c>
-      <c r="C7" t="str">
-        <v>לא רלונטי</v>
-      </c>
-      <c r="D7" t="str">
-        <v>גל מסיקה</v>
-      </c>
-      <c r="E7" t="str">
-        <v>בינדר פראדל</v>
-      </c>
-      <c r="F7" t="str">
-        <v>-</v>
-      </c>
-      <c r="G7" t="str">
-        <v>03.04.2024</v>
-      </c>
-      <c r="H7" t="str">
-        <v>03.04.2024</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>רונן</v>
-      </c>
-      <c r="B8" t="str">
-        <v>גורג</v>
-      </c>
-      <c r="C8" t="str">
-        <v>פרטים</v>
-      </c>
-      <c r="D8" t="str">
-        <v>גל מסיקה</v>
-      </c>
-      <c r="E8" t="str">
-        <v>בינדר פראדל</v>
-      </c>
-      <c r="F8" t="str">
-        <v>-</v>
-      </c>
-      <c r="G8" t="str">
-        <v>04.04.2024</v>
-      </c>
-      <c r="H8" t="str">
-        <v>10.04.2024</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>אברהם</v>
-      </c>
-      <c r="B9" t="str">
-        <v>נגר</v>
-      </c>
-      <c r="C9" t="str">
-        <v>-</v>
-      </c>
-      <c r="D9" t="str">
-        <v>גל מסיקה</v>
-      </c>
-      <c r="E9" t="str">
-        <v>בינדר פראדל</v>
-      </c>
-      <c r="F9" t="str">
-        <v>-</v>
-      </c>
-      <c r="G9" t="str">
-        <v>10.04.2024</v>
-      </c>
-      <c r="H9" t="str">
-        <v>10.04.2024</v>
+        <v>29.05.2024</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>